<commit_message>
py project and maj29 files
</commit_message>
<xml_diff>
--- a/Death per day.xlsx
+++ b/Death per day.xlsx
@@ -410,7 +410,7 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,7 +437,7 @@
         <v>43965</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>43970</v>
+        <v>43972</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
jun26 / every 2 week update
</commit_message>
<xml_diff>
--- a/Death per day.xlsx
+++ b/Death per day.xlsx
@@ -407,10 +407,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B94" activeCellId="0" sqref="B94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I102" activeCellId="0" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -448,6 +448,9 @@
       <c r="I1" s="1" t="n">
         <v>43994</v>
       </c>
+      <c r="J1" s="1" t="n">
+        <v>44008</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -477,6 +480,9 @@
       <c r="I2" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="J2" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -506,6 +512,9 @@
       <c r="I3" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J3" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
@@ -535,6 +544,9 @@
       <c r="I4" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="J4" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -564,6 +576,9 @@
       <c r="I5" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="J5" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -593,6 +608,9 @@
       <c r="I6" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="J6" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -622,6 +640,9 @@
       <c r="I7" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="J7" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -651,6 +672,9 @@
       <c r="I8" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="J8" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -680,6 +704,9 @@
       <c r="I9" s="3" t="n">
         <v>6</v>
       </c>
+      <c r="J9" s="3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -709,6 +736,9 @@
       <c r="I10" s="3" t="n">
         <v>7</v>
       </c>
+      <c r="J10" s="3" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
@@ -738,6 +768,9 @@
       <c r="I11" s="3" t="n">
         <v>9</v>
       </c>
+      <c r="J11" s="3" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
@@ -767,6 +800,9 @@
       <c r="I12" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="J12" s="3" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
@@ -796,6 +832,9 @@
       <c r="I13" s="3" t="n">
         <v>11</v>
       </c>
+      <c r="J13" s="3" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
@@ -825,6 +864,9 @@
       <c r="I14" s="3" t="n">
         <v>11</v>
       </c>
+      <c r="J14" s="3" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
@@ -854,6 +896,9 @@
       <c r="I15" s="3" t="n">
         <v>21</v>
       </c>
+      <c r="J15" s="3" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
@@ -883,6 +928,9 @@
       <c r="I16" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="J16" s="3" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
@@ -912,6 +960,9 @@
       <c r="I17" s="3" t="n">
         <v>31</v>
       </c>
+      <c r="J17" s="3" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
@@ -941,6 +992,9 @@
       <c r="I18" s="3" t="n">
         <v>32</v>
       </c>
+      <c r="J18" s="3" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
@@ -970,6 +1024,9 @@
       <c r="I19" s="3" t="n">
         <v>35</v>
       </c>
+      <c r="J19" s="3" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
@@ -999,6 +1056,9 @@
       <c r="I20" s="3" t="n">
         <v>38</v>
       </c>
+      <c r="J20" s="3" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
@@ -1028,6 +1088,9 @@
       <c r="I21" s="3" t="n">
         <v>45</v>
       </c>
+      <c r="J21" s="3" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
@@ -1057,6 +1120,9 @@
       <c r="I22" s="3" t="n">
         <v>48</v>
       </c>
+      <c r="J22" s="3" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
@@ -1086,6 +1152,9 @@
       <c r="I23" s="3" t="n">
         <v>53</v>
       </c>
+      <c r="J23" s="3" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
@@ -1115,6 +1184,9 @@
       <c r="I24" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="J24" s="3" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
@@ -1144,6 +1216,9 @@
       <c r="I25" s="3" t="n">
         <v>79</v>
       </c>
+      <c r="J25" s="3" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
@@ -1173,6 +1248,9 @@
       <c r="I26" s="3" t="n">
         <v>70</v>
       </c>
+      <c r="J26" s="3" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
@@ -1202,6 +1280,9 @@
       <c r="I27" s="3" t="n">
         <v>86</v>
       </c>
+      <c r="J27" s="3" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
@@ -1231,6 +1312,9 @@
       <c r="I28" s="3" t="n">
         <v>90</v>
       </c>
+      <c r="J28" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
@@ -1260,6 +1344,9 @@
       <c r="I29" s="3" t="n">
         <v>84</v>
       </c>
+      <c r="J29" s="3" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
@@ -1289,6 +1376,9 @@
       <c r="I30" s="3" t="n">
         <v>115</v>
       </c>
+      <c r="J30" s="3" t="n">
+        <v>115</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
@@ -1318,6 +1408,9 @@
       <c r="I31" s="3" t="n">
         <v>86</v>
       </c>
+      <c r="J31" s="3" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
@@ -1347,6 +1440,9 @@
       <c r="I32" s="3" t="n">
         <v>90</v>
       </c>
+      <c r="J32" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
@@ -1376,6 +1472,9 @@
       <c r="I33" s="3" t="n">
         <v>103</v>
       </c>
+      <c r="J33" s="3" t="n">
+        <v>103</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
@@ -1405,6 +1504,9 @@
       <c r="I34" s="3" t="n">
         <v>97</v>
       </c>
+      <c r="J34" s="3" t="n">
+        <v>97</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
@@ -1434,6 +1536,9 @@
       <c r="I35" s="3" t="n">
         <v>85</v>
       </c>
+      <c r="J35" s="3" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
@@ -1463,6 +1568,9 @@
       <c r="I36" s="3" t="n">
         <v>91</v>
       </c>
+      <c r="J36" s="3" t="n">
+        <v>91</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
@@ -1492,6 +1600,9 @@
       <c r="I37" s="3" t="n">
         <v>115</v>
       </c>
+      <c r="J37" s="3" t="n">
+        <v>115</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
@@ -1521,6 +1632,9 @@
       <c r="I38" s="3" t="n">
         <v>111</v>
       </c>
+      <c r="J38" s="3" t="n">
+        <v>111</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
@@ -1550,6 +1664,9 @@
       <c r="I39" s="3" t="n">
         <v>82</v>
       </c>
+      <c r="J39" s="3" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
@@ -1579,6 +1696,9 @@
       <c r="I40" s="3" t="n">
         <v>86</v>
       </c>
+      <c r="J40" s="3" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
@@ -1608,6 +1728,9 @@
       <c r="I41" s="3" t="n">
         <v>88</v>
       </c>
+      <c r="J41" s="3" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
@@ -1637,6 +1760,9 @@
       <c r="I42" s="3" t="n">
         <v>85</v>
       </c>
+      <c r="J42" s="3" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
@@ -1666,6 +1792,9 @@
       <c r="I43" s="3" t="n">
         <v>62</v>
       </c>
+      <c r="J43" s="3" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
@@ -1695,6 +1824,9 @@
       <c r="I44" s="3" t="n">
         <v>77</v>
       </c>
+      <c r="J44" s="3" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
@@ -1722,6 +1854,9 @@
       <c r="I45" s="3" t="n">
         <v>86</v>
       </c>
+      <c r="J45" s="3" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
@@ -1749,6 +1884,9 @@
       <c r="I46" s="3" t="n">
         <v>89</v>
       </c>
+      <c r="J46" s="3" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -1776,6 +1914,9 @@
       <c r="I47" s="3" t="n">
         <v>73</v>
       </c>
+      <c r="J47" s="3" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
@@ -1803,6 +1944,9 @@
       <c r="I48" s="3" t="n">
         <v>75</v>
       </c>
+      <c r="J48" s="3" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
@@ -1830,6 +1974,9 @@
       <c r="I49" s="3" t="n">
         <v>73</v>
       </c>
+      <c r="J49" s="3" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
@@ -1857,6 +2004,9 @@
       <c r="I50" s="3" t="n">
         <v>82</v>
       </c>
+      <c r="J50" s="3" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
@@ -1883,6 +2033,9 @@
       </c>
       <c r="I51" s="3" t="n">
         <v>83</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,6 +2062,9 @@
       <c r="I52" s="3" t="n">
         <v>78</v>
       </c>
+      <c r="J52" s="3" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
@@ -1934,6 +2090,9 @@
       <c r="I53" s="3" t="n">
         <v>78</v>
       </c>
+      <c r="J53" s="3" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
@@ -1959,6 +2118,9 @@
       <c r="I54" s="3" t="n">
         <v>73</v>
       </c>
+      <c r="J54" s="3" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
@@ -1984,6 +2146,9 @@
       <c r="I55" s="3" t="n">
         <v>75</v>
       </c>
+      <c r="J55" s="3" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
@@ -2009,6 +2174,9 @@
       <c r="I56" s="3" t="n">
         <v>84</v>
       </c>
+      <c r="J56" s="3" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
@@ -2034,6 +2202,9 @@
       <c r="I57" s="3" t="n">
         <v>72</v>
       </c>
+      <c r="J57" s="3" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
@@ -2059,6 +2230,9 @@
       <c r="I58" s="3" t="n">
         <v>73</v>
       </c>
+      <c r="J58" s="3" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
@@ -2082,6 +2256,9 @@
         <v>80</v>
       </c>
       <c r="I59" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="J59" s="3" t="n">
         <v>80</v>
       </c>
     </row>
@@ -2107,6 +2284,9 @@
       <c r="I60" s="3" t="n">
         <v>60</v>
       </c>
+      <c r="J60" s="3" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
@@ -2130,6 +2310,9 @@
       <c r="I61" s="3" t="n">
         <v>67</v>
       </c>
+      <c r="J61" s="3" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
@@ -2153,6 +2336,9 @@
       <c r="I62" s="3" t="n">
         <v>74</v>
       </c>
+      <c r="J62" s="3" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
@@ -2176,6 +2362,9 @@
       <c r="I63" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="J63" s="3" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
@@ -2199,6 +2388,9 @@
       <c r="I64" s="3" t="n">
         <v>60</v>
       </c>
+      <c r="J64" s="3" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
@@ -2222,6 +2414,9 @@
       <c r="I65" s="3" t="n">
         <v>51</v>
       </c>
+      <c r="J65" s="3" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
@@ -2243,6 +2438,9 @@
         <v>46</v>
       </c>
       <c r="I66" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="J66" s="3" t="n">
         <v>46</v>
       </c>
     </row>
@@ -2266,6 +2464,9 @@
       <c r="I67" s="3" t="n">
         <v>57</v>
       </c>
+      <c r="J67" s="3" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
@@ -2287,6 +2488,9 @@
       <c r="I68" s="3" t="n">
         <v>48</v>
       </c>
+      <c r="J68" s="3" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
@@ -2308,6 +2512,9 @@
       <c r="I69" s="3" t="n">
         <v>53</v>
       </c>
+      <c r="J69" s="3" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
@@ -2329,6 +2536,9 @@
       <c r="I70" s="3" t="n">
         <v>61</v>
       </c>
+      <c r="J70" s="3" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
@@ -2350,6 +2560,9 @@
       <c r="I71" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="J71" s="3" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
@@ -2367,6 +2580,9 @@
       <c r="I72" s="3" t="n">
         <v>53</v>
       </c>
+      <c r="J72" s="3" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
@@ -2384,6 +2600,9 @@
       <c r="I73" s="3" t="n">
         <v>52</v>
       </c>
+      <c r="J73" s="3" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
@@ -2398,6 +2617,9 @@
       <c r="I74" s="3" t="n">
         <v>54</v>
       </c>
+      <c r="J74" s="3" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
@@ -2412,6 +2634,9 @@
       <c r="I75" s="3" t="n">
         <v>56</v>
       </c>
+      <c r="J75" s="3" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
@@ -2426,6 +2651,9 @@
       <c r="I76" s="3" t="n">
         <v>42</v>
       </c>
+      <c r="J76" s="3" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
@@ -2440,6 +2668,9 @@
       <c r="I77" s="3" t="n">
         <v>41</v>
       </c>
+      <c r="J77" s="3" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
@@ -2454,6 +2685,9 @@
       <c r="I78" s="3" t="n">
         <v>27</v>
       </c>
+      <c r="J78" s="3" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
@@ -2468,6 +2702,9 @@
       <c r="I79" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="J79" s="3" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
@@ -2482,6 +2719,9 @@
       <c r="I80" s="3" t="n">
         <v>38</v>
       </c>
+      <c r="J80" s="3" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
@@ -2496,6 +2736,9 @@
       <c r="I81" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="J81" s="3" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
@@ -2507,6 +2750,9 @@
       <c r="I82" s="3" t="n">
         <v>37</v>
       </c>
+      <c r="J82" s="3" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
@@ -2518,6 +2764,9 @@
       <c r="I83" s="3" t="n">
         <v>43</v>
       </c>
+      <c r="J83" s="3" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
@@ -2529,6 +2778,9 @@
       <c r="I84" s="3" t="n">
         <v>39</v>
       </c>
+      <c r="J84" s="3" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
@@ -2540,6 +2792,9 @@
       <c r="I85" s="3" t="n">
         <v>29</v>
       </c>
+      <c r="J85" s="3" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
@@ -2551,6 +2806,9 @@
       <c r="I86" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="J86" s="3" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
@@ -2562,6 +2820,9 @@
       <c r="I87" s="3" t="n">
         <v>40</v>
       </c>
+      <c r="J87" s="3" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
@@ -2570,6 +2831,9 @@
       <c r="I88" s="3" t="n">
         <v>25</v>
       </c>
+      <c r="J88" s="3" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
@@ -2578,6 +2842,9 @@
       <c r="I89" s="3" t="n">
         <v>13</v>
       </c>
+      <c r="J89" s="3" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
@@ -2586,6 +2853,9 @@
       <c r="I90" s="3" t="n">
         <v>18</v>
       </c>
+      <c r="J90" s="3" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
@@ -2594,6 +2864,9 @@
       <c r="I91" s="3" t="n">
         <v>21</v>
       </c>
+      <c r="J91" s="3" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
@@ -2602,6 +2875,9 @@
       <c r="I92" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="J92" s="3" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
@@ -2610,6 +2886,9 @@
       <c r="I93" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="J93" s="3" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
@@ -2618,6 +2897,9 @@
       <c r="I94" s="3" t="n">
         <v>4</v>
       </c>
+      <c r="J94" s="3" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
@@ -2625,6 +2907,121 @@
       </c>
       <c r="I95" s="3" t="n">
         <v>1</v>
+      </c>
+      <c r="J95" s="3" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="n">
+        <v>43995</v>
+      </c>
+      <c r="J96" s="3" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="n">
+        <v>43996</v>
+      </c>
+      <c r="J97" s="3" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="n">
+        <v>43997</v>
+      </c>
+      <c r="J98" s="3" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="n">
+        <v>43998</v>
+      </c>
+      <c r="J99" s="3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="n">
+        <v>43999</v>
+      </c>
+      <c r="J100" s="3" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="n">
+        <v>44000</v>
+      </c>
+      <c r="J101" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="n">
+        <v>44001</v>
+      </c>
+      <c r="J102" s="3" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="n">
+        <v>44002</v>
+      </c>
+      <c r="J103" s="3" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="n">
+        <v>44003</v>
+      </c>
+      <c r="J104" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="n">
+        <v>44004</v>
+      </c>
+      <c r="J105" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="n">
+        <v>44005</v>
+      </c>
+      <c r="J106" s="3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="n">
+        <v>44006</v>
+      </c>
+      <c r="J107" s="3" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="n">
+        <v>44007</v>
+      </c>
+      <c r="J108" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="n">
+        <v>44008</v>
+      </c>
+      <c r="J109" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>